<commit_message>
Actualizacao do loaddata para trackerentitys
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felizardo Chaguala\Desktop\dhis2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22822BD-8012-41C7-82BF-4AEA2DE57713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CEFDEC-6574-4EC8-8CFB-D2F4DAB998CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9F34BF02-54FC-45FB-A073-5E82DAD013A4}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -465,7 +465,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>